<commit_message>
dict stripping seems to work, however need to test that the merge has all data and then get changesdict working
</commit_message>
<xml_diff>
--- a/public/understanding data files.xlsx
+++ b/public/understanding data files.xlsx
@@ -5,27 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github local repos\Admin_scrape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github local repos\Admin_scrape\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A2E3F804-943B-4FC5-A13F-F441660B97C5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5132AB95-8A65-42A6-90C1-7929068D6EAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8940" windowHeight="6660" xr2:uid="{B465A4E7-1CEA-4E0C-949F-88CC818CDD9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Understanding all my data files</t>
   </si>
@@ -121,6 +126,24 @@
   </si>
   <si>
     <t>Days gap</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T4_dict</t>
+  </si>
+  <si>
+    <t>T4_file</t>
+  </si>
+  <si>
+    <t>T4.html</t>
+  </si>
+  <si>
+    <t>T4_soup</t>
+  </si>
+  <si>
+    <t>mo_T4</t>
   </si>
 </sst>
 </file>
@@ -501,35 +524,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5120D22A-5788-436E-96DC-05EABB6ACE08}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.73046875" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -570,7 +593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -609,7 +632,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -651,7 +674,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -691,6 +714,40 @@
       <c r="N6" s="3">
         <f>M6-M5</f>
         <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="5">
+        <v>43339</v>
+      </c>
+      <c r="N7" s="3">
+        <f>M7-M6</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a naming bug and now changes_dict looks perfect. Progressing to more live testing
</commit_message>
<xml_diff>
--- a/public/understanding data files.xlsx
+++ b/public/understanding data files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github local repos\Admin_scrape\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5132AB95-8A65-42A6-90C1-7929068D6EAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F71804-18D1-463A-B88C-D4FAAB321E2C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8940" windowHeight="6660" xr2:uid="{B465A4E7-1CEA-4E0C-949F-88CC818CDD9C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Understanding all my data files</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>mo_T4</t>
+  </si>
+  <si>
+    <t>D2_backup</t>
+  </si>
+  <si>
+    <t>D2_backup_dict</t>
+  </si>
+  <si>
+    <t>mo_D2_backup</t>
   </si>
 </sst>
 </file>
@@ -524,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5120D22A-5788-436E-96DC-05EABB6ACE08}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -750,6 +759,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3">
+        <v>1134</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1134</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1134</v>
+      </c>
+      <c r="M8" s="5">
+        <v>43339</v>
+      </c>
+      <c r="N8" s="3">
+        <f>M8-M7</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>